<commit_message>
added doubly linked list/node and updated get classroom function
</commit_message>
<xml_diff>
--- a/AllCourses.xlsx
+++ b/AllCourses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mlee.BIGGAR\PycharmProjects\CMPT.395.PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9830B311-EFF4-4209-82E7-3326913BFDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34616772-8D4A-493C-BBAE-63480C9B3610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1470" windowWidth="21900" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4770" yWindow="705" windowWidth="19185" windowHeight="10785" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BCOM" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="BK" sheetId="8" r:id="rId6"/>
     <sheet name="FS" sheetId="9" r:id="rId7"/>
     <sheet name="DXD" sheetId="10" r:id="rId8"/>
+    <sheet name="CLASSROOMS" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="214">
   <si>
     <t>Business Communication (BCOM)</t>
   </si>
@@ -636,6 +637,39 @@
   </si>
   <si>
     <t>DXD Capstone</t>
+  </si>
+  <si>
+    <t>Classroom #</t>
+  </si>
+  <si>
+    <t>Normal Capacity</t>
+  </si>
+  <si>
+    <t>11-533</t>
+  </si>
+  <si>
+    <t>11-534</t>
+  </si>
+  <si>
+    <t>11-560</t>
+  </si>
+  <si>
+    <t>11-562</t>
+  </si>
+  <si>
+    <t>11-564</t>
+  </si>
+  <si>
+    <t>11-458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-430 </t>
+  </si>
+  <si>
+    <t>11-320</t>
+  </si>
+  <si>
+    <t>11-532 Computer Lab</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
@@ -2783,4 +2817,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B207E358-00C2-4DF5-8B0C-7F1646F74870}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added many functionlity/bug fixes. reformatted allcourses
</commit_message>
<xml_diff>
--- a/AllCourses.xlsx
+++ b/AllCourses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mlee.BIGGAR\PycharmProjects\CMPT.395.PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34616772-8D4A-493C-BBAE-63480C9B3610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5D8E71-2C1E-4EC1-A52B-235C18E34C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="705" windowWidth="19185" windowHeight="10785" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BCOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="224">
   <si>
     <t>Business Communication (BCOM)</t>
   </si>
@@ -39,15 +39,9 @@
     <t>PCOM 0203</t>
   </si>
   <si>
-    <t xml:space="preserve"> Effective Professional Writing; Reports~&gt; Proposals~&gt; Plans~&gt; and More.</t>
-  </si>
-  <si>
     <t>SUPR 0751</t>
   </si>
   <si>
-    <t xml:space="preserve">Fundamentals of Management and Supervision (2 hr timeslot) </t>
-  </si>
-  <si>
     <t>PCOM 0204</t>
   </si>
   <si>
@@ -57,69 +51,39 @@
     <t>CMSK 0237</t>
   </si>
   <si>
-    <t xml:space="preserve">Google Suite Essentials (ONLINE ONLY) - Do not schedule immediately before or after other courses. </t>
-  </si>
-  <si>
     <t>SUPR 0837</t>
   </si>
   <si>
-    <t>Building an Engaged Workforce (2 hr timeslot)</t>
-  </si>
-  <si>
     <t>SUPR 0841</t>
   </si>
   <si>
-    <t>Change Management Fundamentals (2 hr timeslot)</t>
-  </si>
-  <si>
     <t>Term 2</t>
   </si>
   <si>
     <t>SUPR 0821</t>
   </si>
   <si>
-    <t>Foundations of Leadership I (2 hr timeslot)</t>
-  </si>
-  <si>
     <t>SUPR 0822</t>
   </si>
   <si>
-    <t>Foundations of Leadership II (2 hr timeslot)</t>
-  </si>
-  <si>
     <t>SUPR 0718</t>
   </si>
   <si>
-    <t xml:space="preserve">Coaching for Performance (2 hr timeslot) </t>
-  </si>
-  <si>
     <t xml:space="preserve">SUPR 0836 </t>
   </si>
   <si>
-    <t xml:space="preserve">Hiring for success (2 hr timeslot) </t>
-  </si>
-  <si>
     <t xml:space="preserve">AVDM 0199 </t>
   </si>
   <si>
-    <t xml:space="preserve">  Digital Marketing  101 - (ONLINE ONLY) - Do not schedule immediately before or after other courses.</t>
-  </si>
-  <si>
     <t>PCOM 0106</t>
   </si>
   <si>
-    <t>Operations Management (2 hr timelslot - schedule for 17 sessions)</t>
-  </si>
-  <si>
     <t>Term 3</t>
   </si>
   <si>
     <t>PCOM 0205</t>
   </si>
   <si>
-    <t xml:space="preserve">Small Businesses and Entrepreneurship in Canada (3 hr timeslots) </t>
-  </si>
-  <si>
     <t>PCOM TBD</t>
   </si>
   <si>
@@ -129,27 +93,15 @@
     <t>PCOM 0207</t>
   </si>
   <si>
-    <t>Developing Your Emotional Intelligence (2hr timeslot)</t>
-  </si>
-  <si>
     <t>SUPR 0863</t>
   </si>
   <si>
-    <t>Design Thinking (2 hr timeslot)</t>
-  </si>
-  <si>
     <t>PCOM 0206</t>
   </si>
   <si>
-    <t xml:space="preserve">Fundamentals of Agile Methdology (3 hr timeslot) </t>
-  </si>
-  <si>
     <t>AVDM 0260</t>
   </si>
   <si>
-    <t xml:space="preserve"> WordPress for Web Page Publishing  Online Only. - Schedule after all classes are done~&gt; end of the term</t>
-  </si>
-  <si>
     <t>Professional Communication (PCOM)</t>
   </si>
   <si>
@@ -168,9 +120,6 @@
     <t>PCOM 0107</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Development I: Microsoft Word~&gt; Excel and Power Point </t>
-  </si>
-  <si>
     <t>CMSK 0233</t>
   </si>
   <si>
@@ -198,9 +147,6 @@
     <t>PCOM 0108</t>
   </si>
   <si>
-    <t>Technical Development II; Microsoft Word~&gt; Excel and Power Point</t>
-  </si>
-  <si>
     <t>PCOM 0202</t>
   </si>
   <si>
@@ -216,36 +162,21 @@
     <t>PCOM 0109</t>
   </si>
   <si>
-    <t>The Job Hunt in Canada The Job Hunt in Canada   (2 hours time slot )</t>
-  </si>
-  <si>
-    <t>Module 1 Resume and Cover Letter: 4 sessions (8hrs) in a LAB - Module 2  Interview Practice: 3 sessions (6hrs) in a classroom</t>
-  </si>
-  <si>
     <t>Project Management (PM)  Courses</t>
   </si>
   <si>
-    <t xml:space="preserve"> Transcript Hours</t>
-  </si>
-  <si>
     <t>PRDV 0201</t>
   </si>
   <si>
     <t xml:space="preserve"> The Basics of Project Management</t>
   </si>
   <si>
-    <t xml:space="preserve">21		</t>
-  </si>
-  <si>
     <t>PRDV 0202</t>
   </si>
   <si>
     <t>Project Scope and Qualit</t>
   </si>
   <si>
-    <t xml:space="preserve">14	</t>
-  </si>
-  <si>
     <t>PRDV 020</t>
   </si>
   <si>
@@ -285,15 +216,9 @@
     <t>PCOM 0131</t>
   </si>
   <si>
-    <t>PM Capstone Project - 13 sessions~&gt; 3 hours each</t>
-  </si>
-  <si>
     <t>Business Analysis (BA)  Courses</t>
   </si>
   <si>
-    <t xml:space="preserve">Transcript Hours	</t>
-  </si>
-  <si>
     <t xml:space="preserve">Term 1	</t>
   </si>
   <si>
@@ -318,9 +243,6 @@
     <t>PRDV 0642</t>
   </si>
   <si>
-    <t>Elicitation and Collaboration 	14</t>
-  </si>
-  <si>
     <t>PRDV 0644</t>
   </si>
   <si>
@@ -348,15 +270,9 @@
     <t>PCOM 0141</t>
   </si>
   <si>
-    <t>BA Capstone Project -  13 sessions~&gt; 3 hours each</t>
-  </si>
-  <si>
     <t>Supply Chain Management &amp; Logistics (GLM)</t>
   </si>
   <si>
-    <t>Transcript Hours</t>
-  </si>
-  <si>
     <t>SCMT 0501</t>
   </si>
   <si>
@@ -378,9 +294,6 @@
     <t>SCMT 9901</t>
   </si>
   <si>
-    <t>International Transport and Trade (Virtual Course with CIFA; No scheduling required)</t>
-  </si>
-  <si>
     <t>SCMT 0503</t>
   </si>
   <si>
@@ -393,9 +306,6 @@
     <t>SCMT 9902</t>
   </si>
   <si>
-    <t>Essentials of Freight Forwarding (Virtual Course with CIFA; No scheduling required)</t>
-  </si>
-  <si>
     <t>SCMT 0505</t>
   </si>
   <si>
@@ -405,12 +315,6 @@
     <t>PCOM 0151</t>
   </si>
   <si>
-    <t>Capstone Project -  13 sessions~&gt; 3 hours each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39			</t>
-  </si>
-  <si>
     <t>BookKeeping Certificate</t>
   </si>
   <si>
@@ -462,24 +366,15 @@
     <t>Integrated Case Studies in Accounting</t>
   </si>
   <si>
-    <t>Foundations of Inventory~&gt; Operations~&gt; Planning and Control</t>
-  </si>
-  <si>
     <t>Full Stack Web Development (FS)</t>
   </si>
   <si>
-    <t>Introduction to Web Development (2 hour timeslots)</t>
-  </si>
-  <si>
     <t>CMSK 0151</t>
   </si>
   <si>
     <t>CMSK 0154</t>
   </si>
   <si>
-    <t>Entity Framework Core Fundamentals (2hour timeslot)</t>
-  </si>
-  <si>
     <t>PCOM 0160</t>
   </si>
   <si>
@@ -489,87 +384,48 @@
     <t>CMSK 0150</t>
   </si>
   <si>
-    <t>HTML/CSS Fundamentals (2 hour timelsots)</t>
-  </si>
-  <si>
     <t>CMSK 0152</t>
   </si>
   <si>
-    <t>Introduction to JavaScript (2 hour timeslots)</t>
-  </si>
-  <si>
     <t xml:space="preserve">CMSK 0151 	</t>
   </si>
   <si>
     <t>CMSK 0157</t>
   </si>
   <si>
-    <t>Introduction to Azure DevOps (2 hour timeslots)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recommended to run at the same time as CMSK0154 (Intro to C#) 	</t>
-  </si>
-  <si>
-    <t>Introduction to C (2 hour timelsots)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recommended to run at the same time as CMSK0157 (Intro to Azure)		</t>
-  </si>
-  <si>
     <t xml:space="preserve">Term 2	</t>
   </si>
   <si>
     <t>CMSK 0153</t>
   </si>
   <si>
-    <t>Introduction to Angular (2 hour timeslot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMSK0151 (HTML/CSS)~&gt; CMSK0152 (JavaScript)~&gt; CMSK0157 (Azure Devops)  	</t>
-  </si>
-  <si>
     <t>CMSK 0200</t>
   </si>
   <si>
-    <t>Advanced C# (2 hour timeslots)</t>
-  </si>
-  <si>
     <t xml:space="preserve">	 CMSK 0154 	</t>
   </si>
   <si>
     <t>CMSK 0201</t>
   </si>
   <si>
-    <t xml:space="preserve">CMSK 0154 and CMSK 0200 	</t>
-  </si>
-  <si>
     <t>CMSK 0203</t>
   </si>
   <si>
     <t>RESTful Web Services using.NETCore (2 hour timeslot)</t>
   </si>
   <si>
-    <t xml:space="preserve">CMSK 0201~&gt; recommend to run the same time as Advanced Angular CMSK202 	</t>
-  </si>
-  <si>
     <t>CMSK 0202</t>
   </si>
   <si>
     <t>Advanced Angular (2 hour timeslot)</t>
   </si>
   <si>
-    <t xml:space="preserve">recommend to run the same time as RESTful Web Services (CMSK203)		</t>
-  </si>
-  <si>
     <t xml:space="preserve">Term 3	</t>
   </si>
   <si>
     <t>Full Stack - Web Development Capstone Project (2 hour timeslot)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ideally~&gt; PCOM 0160 should run AFTER all other courses are completed.   it should be at least 50 hours  as it is co-teach.	</t>
-  </si>
-  <si>
     <t>Digital Experience Design Foundation (DXD)</t>
   </si>
   <si>
@@ -670,13 +526,187 @@
   </si>
   <si>
     <t>11-532 Computer Lab</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Twice/Half</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same time as CMSK0154 (Intro to C#) 	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same time as CMSK0157 (Intro to Azure)		</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMSK 0154, CMSK 0200 	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMSK 0151, CMSK 0152, CMSK 0157	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMSK 0201, same time as CMSK 202 	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same time as CMSK 203	</t>
+  </si>
+  <si>
+    <t>After all other courses are completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Development I: Microsoft Word, Excel and Power Point </t>
+  </si>
+  <si>
+    <t>Technical Development II; Microsoft Word, Excel and Power Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WordPress for Web Page Publishing  Online Only. - Schedule after all classes are done, end of the term</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Effective Professional Writing; Reports, Proposals, Plans, and More.</t>
+  </si>
+  <si>
+    <t>Foundations of Inventory Operations, Planning and Control</t>
+  </si>
+  <si>
+    <t>3 hours each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 hour timeslot </t>
+  </si>
+  <si>
+    <t>Fundamentals of Management and Supervision</t>
+  </si>
+  <si>
+    <t>The Job Hunt in Canada Module 1 Resume and Cover Letter</t>
+  </si>
+  <si>
+    <t>2 hours time slot</t>
+  </si>
+  <si>
+    <t>2 hour timeslot</t>
+  </si>
+  <si>
+    <t>13 sessions</t>
+  </si>
+  <si>
+    <t>PM Capstone Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA Capstone Project </t>
+  </si>
+  <si>
+    <t>Elicitation and Collaboration</t>
+  </si>
+  <si>
+    <t>International Transport and Trade</t>
+  </si>
+  <si>
+    <t>Essentials of Freight Forwarding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capstone Project </t>
+  </si>
+  <si>
+    <t>The Job Hunt in Canada Module 2 Interview Practice</t>
+  </si>
+  <si>
+    <t>3 sessions</t>
+  </si>
+  <si>
+    <t>4 sessions</t>
+  </si>
+  <si>
+    <t>Building an Engaged Workforce</t>
+  </si>
+  <si>
+    <t>Change Management Fundamentals</t>
+  </si>
+  <si>
+    <t>Foundations of Leadership I</t>
+  </si>
+  <si>
+    <t>Foundations of Leadership II</t>
+  </si>
+  <si>
+    <t>Coaching for Performance</t>
+  </si>
+  <si>
+    <t>Hiring for success</t>
+  </si>
+  <si>
+    <t>NBOA</t>
+  </si>
+  <si>
+    <t>Do not schedule immediately before or after other courses.</t>
+  </si>
+  <si>
+    <t>Google Suite Essentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Digital Marketing  101</t>
+  </si>
+  <si>
+    <t>17 sessions</t>
+  </si>
+  <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>3 hour timeslot</t>
+  </si>
+  <si>
+    <t>Small Businesses and Entrepreneurship in Canada</t>
+  </si>
+  <si>
+    <t>Developing Your Emotional Intelligence</t>
+  </si>
+  <si>
+    <t>Fundamentals of Agile Methdology</t>
+  </si>
+  <si>
+    <t>Design Thinking</t>
+  </si>
+  <si>
+    <t>Introduction to Web Development</t>
+  </si>
+  <si>
+    <t>HTML/CSS Fundamentals</t>
+  </si>
+  <si>
+    <t>Introduction to JavaScript</t>
+  </si>
+  <si>
+    <t>Introduction to Azure DevOps</t>
+  </si>
+  <si>
+    <t>Introduction to C</t>
+  </si>
+  <si>
+    <t>Introduction to Angular</t>
+  </si>
+  <si>
+    <t>Advanced C#</t>
+  </si>
+  <si>
+    <t>Entity Framework Core Fundamentals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,6 +837,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1512,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,395 +1559,488 @@
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="95.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="C3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>201</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>203</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>167</v>
+      </c>
+      <c r="H14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>209</v>
       </c>
       <c r="C15">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>212</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>213</v>
       </c>
       <c r="C19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>215</v>
       </c>
       <c r="C20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>214</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="C22">
         <v>6</v>
       </c>
+      <c r="E22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" t="s">
+        <v>210</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+    <col min="2" max="2" width="116.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="C5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>178</v>
       </c>
       <c r="C11">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>185</v>
       </c>
       <c r="C15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1921,139 +2050,146 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="C13">
         <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2064,274 +2200,298 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="C13">
         <v>39</v>
       </c>
+      <c r="F13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="C6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="C9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="C10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="C12">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" t="s">
-        <v>126</v>
+        <v>194</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2341,126 +2501,136 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="C7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C8">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="C9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="C11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="C12">
         <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2470,188 +2640,258 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="99.28515625" customWidth="1"/>
     <col min="4" max="4" width="66" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="C4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="C5">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="C6">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="C9">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="E9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>222</v>
       </c>
       <c r="C10">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>223</v>
       </c>
       <c r="C11">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="C12">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="E12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="C13">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
       <c r="C15">
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>176</v>
+      </c>
+      <c r="E15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2661,157 +2901,187 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="C4">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="C7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="C8">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="C9">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="E9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="C10">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="E10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>150</v>
       </c>
       <c r="C12">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="C13">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="C14">
         <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2823,7 +3093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B207E358-00C2-4DF5-8B0C-7F1646F74870}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2835,15 +3105,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -2851,7 +3121,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="B3">
         <v>36</v>
@@ -2859,7 +3129,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -2867,7 +3137,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2875,7 +3145,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>24</v>
@@ -2883,7 +3153,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -2891,7 +3161,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>163</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -2899,7 +3169,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -2907,7 +3177,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="B10">
         <v>30</v>

</xml_diff>

<commit_message>
Updated node/doublylinked list and getAllPrograms()
</commit_message>
<xml_diff>
--- a/AllCourses.xlsx
+++ b/AllCourses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mlee.BIGGAR\PycharmProjects\CMPT.395.PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5D8E71-2C1E-4EC1-A52B-235C18E34C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5298E118-4B3E-474C-A5D8-6ADC2C1507BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BCOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="220">
   <si>
     <t>Business Communication (BCOM)</t>
   </si>
@@ -594,9 +594,6 @@
     <t>2 hour timeslot</t>
   </si>
   <si>
-    <t>13 sessions</t>
-  </si>
-  <si>
     <t>PM Capstone Project</t>
   </si>
   <si>
@@ -618,12 +615,6 @@
     <t>The Job Hunt in Canada Module 2 Interview Practice</t>
   </si>
   <si>
-    <t>3 sessions</t>
-  </si>
-  <si>
-    <t>4 sessions</t>
-  </si>
-  <si>
     <t>Building an Engaged Workforce</t>
   </si>
   <si>
@@ -652,9 +643,6 @@
   </si>
   <si>
     <t xml:space="preserve">  Digital Marketing  101</t>
-  </si>
-  <si>
-    <t>17 sessions</t>
   </si>
   <si>
     <t>Operations Management</t>
@@ -1550,34 +1538,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="95.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.7265625" customWidth="1"/>
+    <col min="2" max="2" width="95.54296875" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1590,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1613,12 +1601,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -1627,15 +1615,15 @@
         <v>167</v>
       </c>
       <c r="H6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -1644,12 +1632,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1658,17 +1646,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1677,12 +1665,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -1691,12 +1679,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C12">
         <v>7</v>
@@ -1705,12 +1693,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -1719,12 +1707,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1733,15 +1721,15 @@
         <v>167</v>
       </c>
       <c r="H14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C15">
         <v>35</v>
@@ -1749,30 +1737,30 @@
       <c r="F15" t="s">
         <v>187</v>
       </c>
-      <c r="G15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1783,12 +1771,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -1797,12 +1785,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C20">
         <v>7</v>
@@ -1811,21 +1799,21 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1839,7 +1827,7 @@
         <v>167</v>
       </c>
       <c r="H22" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1854,27 +1842,27 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="2" width="116.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="55.1796875" customWidth="1"/>
+    <col min="2" max="2" width="116.7265625" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1885,7 +1873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1896,7 +1884,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1910,7 +1898,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1924,7 +1912,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1938,12 +1926,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1954,7 +1942,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1965,7 +1953,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1979,12 +1967,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1995,7 +1983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2006,7 +1994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2022,16 +2010,16 @@
       <c r="F15" t="s">
         <v>187</v>
       </c>
-      <c r="G15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -2039,8 +2027,8 @@
       <c r="F16" t="s">
         <v>186</v>
       </c>
-      <c r="G16" t="s">
-        <v>196</v>
+      <c r="G16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2053,28 +2041,28 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="57.7265625" customWidth="1"/>
+    <col min="2" max="2" width="76.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2085,7 +2073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2096,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2107,12 +2095,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2123,7 +2111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2134,7 +2122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2148,7 +2136,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2159,12 +2147,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2175,12 +2163,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C13">
         <v>39</v>
@@ -2188,8 +2176,8 @@
       <c r="F13" t="s">
         <v>182</v>
       </c>
-      <c r="G13" t="s">
-        <v>188</v>
+      <c r="G13">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2202,28 +2190,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="38.1796875" customWidth="1"/>
+    <col min="2" max="2" width="70.1796875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2234,7 +2222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -2245,7 +2233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -2256,23 +2244,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -2283,7 +2271,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2294,7 +2282,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -2308,12 +2296,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -2324,12 +2312,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13">
         <v>39</v>
@@ -2337,8 +2325,8 @@
       <c r="F13" t="s">
         <v>182</v>
       </c>
-      <c r="G13" t="s">
-        <v>188</v>
+      <c r="G13">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2351,29 +2339,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="72.42578125" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="72.453125" customWidth="1"/>
+    <col min="2" max="2" width="60.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2384,7 +2373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -2395,7 +2384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -2406,12 +2395,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -2420,12 +2409,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -2436,7 +2425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -2447,12 +2436,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -2461,12 +2450,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -2477,12 +2466,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13">
         <v>39</v>
@@ -2490,8 +2479,8 @@
       <c r="F13" t="s">
         <v>182</v>
       </c>
-      <c r="G13" t="s">
-        <v>188</v>
+      <c r="G13">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2503,27 +2492,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="79" customWidth="1"/>
-    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -2534,7 +2523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2545,7 +2534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -2556,12 +2545,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2572,7 +2561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2586,7 +2575,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -2600,12 +2589,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -2619,7 +2608,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -2642,19 +2631,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="99.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="2" max="2" width="99.26953125" customWidth="1"/>
     <col min="4" max="4" width="66" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -2662,17 +2651,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -2684,12 +2673,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -2701,12 +2690,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -2721,12 +2710,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -2741,12 +2730,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -2761,20 +2750,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>121</v>
       </c>
-      <c r="E8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C9">
         <v>18</v>
@@ -2789,12 +2775,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -2809,12 +2795,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C11">
         <v>18</v>
@@ -2829,7 +2815,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2849,7 +2835,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -2869,12 +2855,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -2904,28 +2890,28 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.7265625" customWidth="1"/>
+    <col min="2" max="2" width="37.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="47.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2939,7 +2925,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -2953,7 +2939,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -2970,12 +2956,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2989,7 +2975,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -3003,7 +2989,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3020,7 +3006,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3037,12 +3023,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -3056,7 +3042,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -3070,7 +3056,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -3097,13 +3083,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>155</v>
       </c>
@@ -3111,7 +3097,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3119,7 +3105,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -3127,7 +3113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -3135,7 +3121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -3143,7 +3129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -3151,7 +3137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -3159,7 +3145,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -3167,7 +3153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -3175,7 +3161,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>165</v>
       </c>

</xml_diff>